<commit_message>
Added LM to Train Data
</commit_message>
<xml_diff>
--- a/TrainData.xlsx
+++ b/TrainData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajin\Desktop\akshay project files\Machine Learning\Decision Tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajin\Desktop\machine_learning\Machine-Learning-Decision_Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DD7388-FE37-4956-9B0F-634C14B081AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C4B828-F45A-453C-84A4-AE93B697CA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>values</t>
   </si>
@@ -41,6 +41,69 @@
   </si>
   <si>
     <t>Sl.no</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>Lm1</t>
+  </si>
+  <si>
+    <t>Lm2</t>
+  </si>
+  <si>
+    <t>Lm3</t>
+  </si>
+  <si>
+    <t>Lm4</t>
+  </si>
+  <si>
+    <t>Lm5</t>
+  </si>
+  <si>
+    <t>Lm6</t>
+  </si>
+  <si>
+    <t>Lm7</t>
+  </si>
+  <si>
+    <t>Lm8</t>
+  </si>
+  <si>
+    <t>Lm9</t>
+  </si>
+  <si>
+    <t>Lm10</t>
+  </si>
+  <si>
+    <t>Lm11</t>
+  </si>
+  <si>
+    <t>Lm12</t>
+  </si>
+  <si>
+    <t>Lm13</t>
+  </si>
+  <si>
+    <t>Lm14</t>
+  </si>
+  <si>
+    <t>Lm15</t>
+  </si>
+  <si>
+    <t>Lm16</t>
+  </si>
+  <si>
+    <t>Lm17</t>
+  </si>
+  <si>
+    <t>Lm18</t>
+  </si>
+  <si>
+    <t>Lm19</t>
+  </si>
+  <si>
+    <t>Lm20</t>
   </si>
 </sst>
 </file>
@@ -389,246 +452,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="21.90625" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>2.3449999999999999E-2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>5.6869999999999997E-2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>3.4209999999999997E-2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
         <v>1.435E-2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>6.4229999999999995E-2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
         <v>8.4650000000000003E-2</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
         <v>1.325E-2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
         <v>9.2530000000000001E-2</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
         <v>6.2429999999999999E-2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
         <v>4.3150000000000001E-2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
         <v>0.13525999999999999</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
         <v>7.6450000000000004E-2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
         <v>8.7150000000000005E-2</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
         <v>3.4909999999999997E-2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
         <v>0.19461999999999999</v>
       </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
         <v>0.17652000000000001</v>
       </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
         <v>9.0230000000000005E-2</v>
       </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
         <v>0.22341</v>
       </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
         <v>6.5100000000000002E-3</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
         <v>6.1530000000000001E-2</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed LM to int
</commit_message>
<xml_diff>
--- a/TrainData.xlsx
+++ b/TrainData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajin\Desktop\machine_learning\Machine-Learning-Decision_Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C4B828-F45A-453C-84A4-AE93B697CA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CF2836-ACA2-4754-B96C-BFF79110B89F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
   <si>
     <t>values</t>
   </si>
@@ -44,66 +44,6 @@
   </si>
   <si>
     <t>LM</t>
-  </si>
-  <si>
-    <t>Lm1</t>
-  </si>
-  <si>
-    <t>Lm2</t>
-  </si>
-  <si>
-    <t>Lm3</t>
-  </si>
-  <si>
-    <t>Lm4</t>
-  </si>
-  <si>
-    <t>Lm5</t>
-  </si>
-  <si>
-    <t>Lm6</t>
-  </si>
-  <si>
-    <t>Lm7</t>
-  </si>
-  <si>
-    <t>Lm8</t>
-  </si>
-  <si>
-    <t>Lm9</t>
-  </si>
-  <si>
-    <t>Lm10</t>
-  </si>
-  <si>
-    <t>Lm11</t>
-  </si>
-  <si>
-    <t>Lm12</t>
-  </si>
-  <si>
-    <t>Lm13</t>
-  </si>
-  <si>
-    <t>Lm14</t>
-  </si>
-  <si>
-    <t>Lm15</t>
-  </si>
-  <si>
-    <t>Lm16</t>
-  </si>
-  <si>
-    <t>Lm17</t>
-  </si>
-  <si>
-    <t>Lm18</t>
-  </si>
-  <si>
-    <t>Lm19</t>
-  </si>
-  <si>
-    <t>Lm20</t>
   </si>
 </sst>
 </file>
@@ -454,7 +394,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -480,8 +422,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>2.3449999999999999E-2</v>
@@ -494,8 +436,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>5.6869999999999997E-2</v>
@@ -508,8 +450,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="B4">
+        <v>3</v>
       </c>
       <c r="C4">
         <v>3.4209999999999997E-2</v>
@@ -522,8 +464,8 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
+      <c r="B5">
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1.435E-2</v>
@@ -536,8 +478,8 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
+      <c r="B6">
+        <v>5</v>
       </c>
       <c r="C6">
         <v>6.4229999999999995E-2</v>
@@ -550,8 +492,8 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
+      <c r="B7">
+        <v>6</v>
       </c>
       <c r="C7">
         <v>8.4650000000000003E-2</v>
@@ -564,8 +506,8 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
+      <c r="B8">
+        <v>7</v>
       </c>
       <c r="C8">
         <v>1.325E-2</v>
@@ -578,8 +520,8 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
+      <c r="B9">
+        <v>8</v>
       </c>
       <c r="C9">
         <v>9.2530000000000001E-2</v>
@@ -592,8 +534,8 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
+      <c r="B10">
+        <v>9</v>
       </c>
       <c r="C10">
         <v>6.2429999999999999E-2</v>
@@ -606,8 +548,8 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>16</v>
+      <c r="B11">
+        <v>10</v>
       </c>
       <c r="C11">
         <v>4.3150000000000001E-2</v>
@@ -620,8 +562,8 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
+      <c r="B12">
+        <v>11</v>
       </c>
       <c r="C12">
         <v>0.13525999999999999</v>
@@ -634,8 +576,8 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
+      <c r="B13">
+        <v>12</v>
       </c>
       <c r="C13">
         <v>7.6450000000000004E-2</v>
@@ -648,8 +590,8 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>19</v>
+      <c r="B14">
+        <v>13</v>
       </c>
       <c r="C14">
         <v>8.7150000000000005E-2</v>
@@ -662,8 +604,8 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>20</v>
+      <c r="B15">
+        <v>14</v>
       </c>
       <c r="C15">
         <v>3.4909999999999997E-2</v>
@@ -676,8 +618,8 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>21</v>
+      <c r="B16">
+        <v>15</v>
       </c>
       <c r="C16">
         <v>0.19461999999999999</v>
@@ -690,8 +632,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>22</v>
+      <c r="B17">
+        <v>16</v>
       </c>
       <c r="C17">
         <v>0.17652000000000001</v>
@@ -704,8 +646,8 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>23</v>
+      <c r="B18">
+        <v>17</v>
       </c>
       <c r="C18">
         <v>9.0230000000000005E-2</v>
@@ -718,8 +660,8 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>24</v>
+      <c r="B19">
+        <v>18</v>
       </c>
       <c r="C19">
         <v>0.22341</v>
@@ -732,8 +674,8 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>25</v>
+      <c r="B20">
+        <v>19</v>
       </c>
       <c r="C20">
         <v>6.5100000000000002E-3</v>
@@ -746,8 +688,8 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>26</v>
+      <c r="B21">
+        <v>20</v>
       </c>
       <c r="C21">
         <v>6.1530000000000001E-2</v>

</xml_diff>

<commit_message>
Changes made to Train Data
</commit_message>
<xml_diff>
--- a/TrainData.xlsx
+++ b/TrainData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajin\Desktop\machine_learning\Machine-Learning-Decision_Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED91CAD5-36C7-4639-8AA3-ADB22BD284F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F302AC4-7D32-4E24-98E0-F815F6225A37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,7 +499,7 @@
         <v>8.4650000000000003E-2</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -527,7 +527,7 @@
         <v>9.2530000000000001E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -597,7 +597,7 @@
         <v>8.7150000000000005E-2</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -653,7 +653,7 @@
         <v>9.0230000000000005E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added more train data
</commit_message>
<xml_diff>
--- a/TrainData.xlsx
+++ b/TrainData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajin\Desktop\machine_learning\Machine-Learning-Decision_Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE9C089-47E2-4353-BF90-46D2F5B6D720}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD383ADC-1B4A-4156-89EA-08C2014C2B8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="7">
   <si>
     <t>class</t>
   </si>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -696,6 +696,426 @@
         <v>6.1530000000000001E-2</v>
       </c>
       <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>5.2139999999999999E-2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>2.215E-2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>0.15564</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>0.18546000000000001</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>7.4560000000000001E-2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>8.4309999999999996E-2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>0.21543000000000001</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>5.1200000000000004E-3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>4.1520000000000001E-2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>0.12453</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>6.4449999999999993E-2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>7.7539999999999998E-2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>9.4539999999999999E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>4.2250000000000003E-2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>3.4450000000000001E-2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>5.2310000000000002E-2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>7.3349999999999999E-2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>0.24156</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>9.5560000000000006E-2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>0.12411999999999999</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>1.521E-2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>4.1140000000000003E-2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>5.1240000000000001E-2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>9.0240000000000001E-2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>0.34151999999999999</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>7.5410000000000005E-2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>2.4150000000000001E-2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>4.215E-2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>6.1240000000000003E-2</v>
+      </c>
+      <c r="D51" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed certain values in train data
</commit_message>
<xml_diff>
--- a/TrainData.xlsx
+++ b/TrainData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajin\Desktop\machine_learning\Machine-Learning-Decision_Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD383ADC-1B4A-4156-89EA-08C2014C2B8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3772D8-5D61-46FC-BB83-CDD490C2F6DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -875,7 +875,7 @@
         <v>33</v>
       </c>
       <c r="C34">
-        <v>9.4539999999999999E-2</v>
+        <v>0.11024</v>
       </c>
       <c r="D34" t="s">
         <v>2</v>
@@ -987,7 +987,7 @@
         <v>41</v>
       </c>
       <c r="C42">
-        <v>0.12411999999999999</v>
+        <v>0.11244999999999999</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>

</xml_diff>